<commit_message>
Upadated wrong input handling
</commit_message>
<xml_diff>
--- a/ExcelDemo.xlsx
+++ b/ExcelDemo.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32">
   <si>
     <t>Id</t>
   </si>
@@ -68,7 +68,7 @@
     <t>abc123</t>
   </si>
   <si>
-    <t>Cod</t>
+    <t>Netbanking</t>
   </si>
   <si>
     <t>Suresh</t>
@@ -80,7 +80,7 @@
     <t>Silver</t>
   </si>
   <si>
-    <t xml:space="preserve"> Netbanking</t>
+    <t>CreditCard</t>
   </si>
   <si>
     <t>Paresh</t>
@@ -92,21 +92,18 @@
     <t>Platinum</t>
   </si>
   <si>
-    <t>No</t>
-  </si>
-  <si>
     <t>abc1234</t>
   </si>
   <si>
-    <t>CreditCard</t>
-  </si>
-  <si>
     <t>Nitin</t>
   </si>
   <si>
     <t>solanki</t>
   </si>
   <si>
+    <t>Goldefgdfg</t>
+  </si>
+  <si>
     <t>Mukesh</t>
   </si>
   <si>
@@ -114,9 +111,6 @@
   </si>
   <si>
     <t>abc142</t>
-  </si>
-  <si>
-    <t>Netbanking</t>
   </si>
 </sst>
 </file>
@@ -124,10 +118,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -157,6 +151,28 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
@@ -165,8 +181,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -180,16 +197,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -197,14 +215,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -233,14 +243,36 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -250,45 +282,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -316,55 +310,151 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -376,31 +466,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -412,85 +484,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -523,6 +517,15 @@
       <right/>
       <top/>
       <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -543,6 +546,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -554,35 +566,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -601,12 +584,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -618,136 +615,133 @@
     <xf numFmtId="179" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1086,12 +1080,13 @@
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="5"/>
   <cols>
     <col min="4" max="4" width="17.7142857142857" customWidth="1"/>
+    <col min="5" max="5" width="9.57142857142857"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -1143,10 +1138,10 @@
         <v>13</v>
       </c>
       <c r="E2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>156456</v>
       </c>
       <c r="G2" t="s">
         <v>14</v>
@@ -1216,19 +1211,19 @@
         <v>2</v>
       </c>
       <c r="F4">
-        <v>8453</v>
+        <v>0</v>
       </c>
       <c r="G4" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="H4" t="s">
         <v>15</v>
       </c>
       <c r="I4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J4" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="K4">
         <v>3333</v>
@@ -1239,13 +1234,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" t="s">
         <v>28</v>
-      </c>
-      <c r="C5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D5" t="s">
-        <v>13</v>
       </c>
       <c r="E5">
         <v>4</v>
@@ -1254,7 +1249,7 @@
         <v>47689</v>
       </c>
       <c r="G5" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="H5" t="s">
         <v>15</v>
@@ -1263,7 +1258,7 @@
         <v>16</v>
       </c>
       <c r="J5" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="K5">
         <v>4444</v>
@@ -1274,13 +1269,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" t="s">
         <v>30</v>
       </c>
-      <c r="C6" t="s">
-        <v>31</v>
-      </c>
       <c r="D6" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E6">
         <v>2</v>
@@ -1295,10 +1290,10 @@
         <v>15</v>
       </c>
       <c r="I6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J6" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="K6">
         <v>5555</v>

</xml_diff>

<commit_message>
Seat availability functionality added
</commit_message>
<xml_diff>
--- a/ExcelDemo.xlsx
+++ b/ExcelDemo.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31">
   <si>
     <t>Id</t>
   </si>
@@ -99,9 +99,6 @@
   </si>
   <si>
     <t>solanki</t>
-  </si>
-  <si>
-    <t>Goldefgdfg</t>
   </si>
   <si>
     <t>Mukesh</t>
@@ -118,10 +115,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -151,25 +148,25 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -183,38 +180,23 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -229,6 +211,22 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -244,6 +242,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -251,45 +256,37 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -304,31 +301,151 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -340,151 +457,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -498,17 +495,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -518,15 +509,6 @@
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -546,11 +528,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -570,6 +558,26 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -584,23 +592,15 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -612,136 +612,133 @@
     <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1080,13 +1077,15 @@
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="5"/>
   <cols>
     <col min="4" max="4" width="17.7142857142857" customWidth="1"/>
     <col min="5" max="5" width="9.57142857142857"/>
+    <col min="6" max="6" width="10.5714285714286"/>
+    <col min="8" max="8" width="13.5714285714286" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -1138,10 +1137,10 @@
         <v>13</v>
       </c>
       <c r="E2">
-        <v>4</v>
+        <v>99</v>
       </c>
       <c r="F2">
-        <v>156456</v>
+        <v>41566</v>
       </c>
       <c r="G2" t="s">
         <v>14</v>
@@ -1208,10 +1207,10 @@
         <v>24</v>
       </c>
       <c r="E4">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>165464</v>
       </c>
       <c r="G4" t="s">
         <v>14</v>
@@ -1240,10 +1239,10 @@
         <v>27</v>
       </c>
       <c r="D5" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="E5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F5">
         <v>47689</v>
@@ -1269,16 +1268,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" t="s">
         <v>29</v>
-      </c>
-      <c r="C6" t="s">
-        <v>30</v>
       </c>
       <c r="D6" t="s">
         <v>20</v>
       </c>
       <c r="E6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F6">
         <v>45689</v>
@@ -1290,7 +1289,7 @@
         <v>15</v>
       </c>
       <c r="I6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J6" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
Added some exception handled cases
</commit_message>
<xml_diff>
--- a/ExcelDemo.xlsx
+++ b/ExcelDemo.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="0">
   <si>
     <t>Id</t>
   </si>
@@ -60,27 +60,36 @@
     <t>Gold</t>
   </si>
   <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>abc1234</t>
+  </si>
+  <si>
+    <t>NetBanking</t>
+  </si>
+  <si>
+    <t>Suresh</t>
+  </si>
+  <si>
+    <t>Verma</t>
+  </si>
+  <si>
+    <t>Silvere</t>
+  </si>
+  <si>
     <t>Yes</t>
   </si>
   <si>
-    <t>Login</t>
+    <t>SignUp</t>
   </si>
   <si>
     <t>abc123</t>
   </si>
   <si>
-    <t>NetBanking</t>
-  </si>
-  <si>
-    <t>Suresh</t>
-  </si>
-  <si>
-    <t>Verma</t>
-  </si>
-  <si>
-    <t>Silver</t>
-  </si>
-  <si>
     <t>CreditCard</t>
   </si>
   <si>
@@ -102,9 +111,6 @@
     <t>Mukesh</t>
   </si>
   <si>
-    <t>Gandhi</t>
-  </si>
-  <si>
     <t>abc142</t>
   </si>
   <si>
@@ -120,40 +126,43 @@
     <t>Time</t>
   </si>
   <si>
-    <t>20020.0</t>
+    <t>4520.0</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>6:00</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>820.0</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>Revenue:</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>60</t>
+  </si>
+  <si>
+    <t>80</t>
   </si>
   <si>
     <t>100</t>
-  </si>
-  <si>
-    <t>6:00</t>
-  </si>
-  <si>
-    <t>920.0</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>4520.0</t>
-  </si>
-  <si>
-    <t>15</t>
-  </si>
-  <si>
-    <t>Revenue:</t>
-  </si>
-  <si>
-    <t>60</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>0</t>
   </si>
 </sst>
 </file>
@@ -161,10 +170,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -175,8 +184,69 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -189,32 +259,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -237,67 +299,6 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -313,7 +314,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -328,187 +337,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -519,15 +528,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -542,6 +542,30 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -572,39 +596,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -619,151 +610,169 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="14" fontId="2" numFmtId="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="8" fontId="10" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="176">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="177">
       <alignment vertical="center"/>
     </xf>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="178">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="176">
-      <alignment vertical="center"/>
-    </xf>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="179">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="177">
-      <alignment vertical="center"/>
-    </xf>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="9">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="3" fillId="8" fontId="6" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="1" fillId="0" fontId="3" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyFont="0" applyNumberFormat="0" applyProtection="0" borderId="2" fillId="7" fontId="0" numFmtId="0">
+    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="4" fillId="5" fontId="7" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="2" fillId="0" fontId="4" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyFont="0" applyNumberFormat="0" applyProtection="0" borderId="1" fillId="2" fontId="0" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="11" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="11" fontId="8" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="12" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="14" fontId="10" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="13" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="19" fontId="1" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="15" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="6" fontId="2" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="19" numFmtId="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="16" fontId="10" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="17" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="2" fillId="0" fontId="3" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="8" fillId="0" fontId="6" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="6" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="3" fillId="4" fontId="5" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="22" fontId="8" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="7" fontId="9" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="6" fillId="19" fontId="16" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="24" fontId="10" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="3" fillId="19" fontId="19" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="7" fillId="0" fontId="18" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="5" fillId="0" fontId="14" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
     <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="3" fontId="2" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="5" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="18" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="1" fillId="0" fontId="14" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="5" fillId="0" fontId="9" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="9" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="6" fillId="17" fontId="12" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="24" fontId="1" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="5" fontId="4" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="8" fillId="13" fontId="17" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="16" fontId="2" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="6" fillId="13" fontId="10" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="7" fillId="0" fontId="16" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="4" fillId="0" fontId="7" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="15" fontId="11" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="11" fontId="8" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="10" fontId="1" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="26" fontId="2" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="2" fontId="1" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="9" fontId="1" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="12" fontId="2" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="27" fontId="2" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="21" fontId="1" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="20" fontId="1" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="22" fontId="2" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="29" fontId="1" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="30" fontId="2" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="25" fontId="2" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="18" fontId="1" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="23" fontId="2" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="31" fontId="1" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="32" fontId="1" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="28" fontId="2" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="4" fontId="1" numFmtId="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="18" fontId="15" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="20" fontId="8" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="26" fontId="10" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="23" fontId="8" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="15" fontId="8" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="13" fontId="10" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="25" fontId="10" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="6" fontId="8" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="17" fontId="8" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="12" fontId="10" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="28" fontId="8" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="29" fontId="10" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="31" fontId="10" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="32" fontId="8" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="30" fontId="10" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="21" fontId="8" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="27" fontId="8" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="10" fontId="10" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="9" fontId="8" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2376,10 +2385,13 @@
   <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="5"/>
+  <cols>
+    <col min="5" max="5" width="9.57142857142857" collapsed="false"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" t="s">
@@ -2430,10 +2442,10 @@
         <v>13</v>
       </c>
       <c r="E2">
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>15416</v>
       </c>
       <c r="G2" t="s">
         <v>14</v>
@@ -2465,22 +2477,22 @@
         <v>20</v>
       </c>
       <c r="E3">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>4744</v>
       </c>
       <c r="G3" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="H3" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="I3" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="J3" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="K3">
         <v>2222</v>
@@ -2491,22 +2503,22 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D4" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E4">
         <v>15</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>442</v>
       </c>
       <c r="G4" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="H4" t="s">
         <v>15</v>
@@ -2526,34 +2538,34 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C5" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D5" t="s">
         <v>13</v>
       </c>
       <c r="E5">
-        <v>66</v>
+        <v>9</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>4255</v>
       </c>
       <c r="G5" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="H5" t="s">
         <v>15</v>
       </c>
       <c r="I5" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="J5" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="K5">
-        <v>4444</v>
+        <v>5555</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -2561,31 +2573,31 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C6" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="D6" t="s">
         <v>13</v>
       </c>
       <c r="E6">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <v>15636</v>
       </c>
       <c r="G6" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="H6" t="s">
         <v>15</v>
       </c>
       <c r="I6" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="J6" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="K6">
         <v>5555</v>
@@ -2601,97 +2613,131 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <sheetPr/>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="4" outlineLevelRow="4"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="4" outlineLevelRow="6"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" t="s">
         <v>41</v>
       </c>
-      <c r="B2" t="s">
+      <c r="E3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" t="s">
         <v>45</v>
       </c>
-      <c r="C2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" t="s">
-        <v>39</v>
-      </c>
-      <c r="D4" t="s">
-        <v>40</v>
-      </c>
       <c r="E4" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" t="s">
+        <v>45</v>
+      </c>
+      <c r="E5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
         <v>42</v>
       </c>
-      <c r="C5" t="s">
-        <v>43</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="B6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" t="s">
         <v>44</v>
       </c>
-      <c r="E5" t="s">
+      <c r="D6" t="s">
+        <v>45</v>
+      </c>
+      <c r="E6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" t="s">
         <v>44</v>
+      </c>
+      <c r="D7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E7" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>